<commit_message>
Add mechanical layer and update part list
</commit_message>
<xml_diff>
--- a/ADC_PWM_Board/ADC_PWM_Board - MDP/WDY_ADC_PWM_Board_Part_List.xlsx
+++ b/ADC_PWM_Board/ADC_PWM_Board - MDP/WDY_ADC_PWM_Board_Part_List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\ExMachina\repos\WDY-electronics\ADC_PWM_Board\ADC_PWM_Board - Fabrication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\ExMachina\repos\WDY-electronics\ADC_PWM_Board\ADC_PWM_Board - MDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,9 +15,6 @@
     <sheet name="PdG" sheetId="2" r:id="rId1"/>
     <sheet name="BOM" sheetId="1" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
   <si>
     <t>Value</t>
   </si>
@@ -208,6 +205,48 @@
   </si>
   <si>
     <t>Operational Amplifier</t>
+  </si>
+  <si>
+    <t>MPN</t>
+  </si>
+  <si>
+    <t>22-05-7028</t>
+  </si>
+  <si>
+    <t>22-05-7038</t>
+  </si>
+  <si>
+    <t>22-05-7048</t>
+  </si>
+  <si>
+    <t>22-05-7058</t>
+  </si>
+  <si>
+    <t>MC0603B104K250CT</t>
+  </si>
+  <si>
+    <t>MCMR06X1002FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X1801FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X1001FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X1201FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X1000FTL</t>
+  </si>
+  <si>
+    <t>HCPL-0631-500E</t>
+  </si>
+  <si>
+    <t>TLV313IDBVT</t>
+  </si>
+  <si>
+    <t>MCMR06X2701FTL</t>
   </si>
 </sst>
 </file>
@@ -258,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -279,11 +318,20 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -396,18 +444,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F16" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:F16"/>
-  <sortState ref="A2:F16">
-    <sortCondition ref="E1:E16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G16"/>
+  <sortState ref="A2:G16">
+    <sortCondition ref="C1:C16"/>
   </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Qty" dataDxfId="7"/>
-    <tableColumn id="2" name="Value" dataDxfId="6"/>
-    <tableColumn id="3" name="Device" dataDxfId="5"/>
-    <tableColumn id="4" name="Package" dataDxfId="4"/>
-    <tableColumn id="5" name="Parts" dataDxfId="3"/>
-    <tableColumn id="6" name="Description" dataDxfId="2"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Qty" dataDxfId="6"/>
+    <tableColumn id="2" name="Value" dataDxfId="5"/>
+    <tableColumn id="3" name="Device" dataDxfId="4"/>
+    <tableColumn id="4" name="Package" dataDxfId="3"/>
+    <tableColumn id="5" name="Parts" dataDxfId="2"/>
+    <tableColumn id="6" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" name="MPN" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -760,7 +809,7 @@
       </c>
       <c r="B10" s="3">
         <f ca="1">TODAY()</f>
-        <v>42759</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -784,8 +833,8 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +844,7 @@
     <col min="4" max="4" width="19.7109375" style="6" customWidth="1"/>
     <col min="5" max="5" width="33" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" style="6" customWidth="1"/>
     <col min="9" max="9" width="12.140625" style="6" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" style="6" customWidth="1"/>
@@ -831,7 +880,9 @@
       <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -839,24 +890,26 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D2" s="8">
+        <v>2007041</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -867,46 +920,50 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2007041</v>
+        <v>23</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2007069</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="4"/>
+      <c r="A4" s="4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2007100</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -914,24 +971,26 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="7">
-        <v>2007100</v>
+        <v>36</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2007130</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -939,74 +998,80 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="7">
-        <v>2007069</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="6">
         <v>1</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="7">
-        <v>2007130</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="4"/>
+      <c r="B7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>2</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="4"/>
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1757242</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1031,7 +1096,9 @@
       <c r="F9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -1039,10 +1106,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>18</v>
@@ -1051,12 +1118,14 @@
         <v>5</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -1064,24 +1133,26 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -1089,22 +1160,25 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>21</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1112,7 +1186,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>18</v>
@@ -1121,30 +1195,36 @@
         <v>5</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="G13" s="6" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>1</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>59</v>
+      <c r="A14" s="4">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1152,19 +1232,22 @@
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>58</v>
+        <v>43</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1172,24 +1255,30 @@
         <v>1</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="94" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="73" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;F</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>